<commit_message>
update: solutions, ex pt2, risk article
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/PM2/econ/week2/exercises.xlsx
+++ b/PM2/econ/week2/exercises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\pm\PM2\econ\week2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12989B83-12FF-44D5-A70F-D5F1903247F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01A87F4-21A7-421A-869C-214DFE0B4F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D9D185C7-CA61-44DF-8BA3-8C674C348F4C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D9D185C7-CA61-44DF-8BA3-8C674C348F4C}"/>
   </bookViews>
   <sheets>
     <sheet name="class" sheetId="1" r:id="rId1"/>
@@ -118,8 +118,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000000000000000%"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
-    <numFmt numFmtId="169" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -196,8 +196,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1710,7 +1710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B462CFD6-C60A-4BAB-B1E7-8375DF5C63FA}">
   <dimension ref="A3:AB69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A64" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
@@ -2330,7 +2330,7 @@
         <v>2379.6945203819337</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:E34" si="1">D33*(1+$B$32)^($X$32-D32)</f>
+        <f t="shared" ref="D34" si="1">D33*(1+$B$32)^($X$32-D32)</f>
         <v>0</v>
       </c>
       <c r="E34">
@@ -2761,7 +2761,7 @@
         <v>25169.168576786255</v>
       </c>
       <c r="H56">
-        <f t="shared" ref="G56:AB56" si="4">H55*(1+$B$54)^($AB$54-H54)</f>
+        <f t="shared" ref="H56:AB56" si="4">H55*(1+$B$54)^($AB$54-H54)</f>
         <v>23304.785719246531</v>
       </c>
       <c r="I56">
@@ -3201,10 +3201,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9334CB-CB25-4C95-B5F5-EF03A8F375BB}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3449,10 +3449,162 @@
         <v>6.6574999196526985E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <f>B32*100</f>
         <v>6.6574999196526985</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f>11.76/12</f>
+        <v>0.98</v>
+      </c>
+      <c r="C35">
+        <f>30000*(1+0.0098)^9</f>
+        <v>32752.130213280256</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f>54000*(1+0.0098)</f>
+        <v>54529.200000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f>C35+C36</f>
+        <v>87281.330213280264</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <f>60000*(1+0.0098)^(4)</f>
+        <v>62386.800839500916</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f>C37-C38</f>
+        <v>24894.529373779347</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f>16.56/360</f>
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f>46000*(1+0.00046)^(65)+63000*(1+0.00046)^(135)+76000</f>
+        <v>190431.21670183135</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <f>(1+0.00046)^(24)+(2/(1+0.00046)^(68))</f>
+        <v>2.9495208563753668</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <f>B43/B44</f>
+        <v>64563.441309531932</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <f>B45*3</f>
+        <v>193690.32392859581</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <f>21.84/12</f>
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <f>12000*(1+0.0182)^(5)+7500*(1+0.0182)^(2)</f>
+        <v>20907.963135319085</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <f>B50-10000</f>
+        <v>10907.963135319085</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <f>B51*(1+0.0182)^2</f>
+        <v>11308.626147153642</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <f>B51*(1+0.0182)^(2)</f>
+        <v>11308.626147153642</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <f>7.56/360</f>
+        <v>2.0999999999999998E-2</v>
+      </c>
+      <c r="C56">
+        <f>16800*(1+0.00021)^(67)</f>
+        <v>17038.021564079383</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <f>25600+C56</f>
+        <v>42638.021564079383</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <f>C57*(1+0.00021)^(25)</f>
+        <v>42862.436187568717</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <f>C58-20000</f>
+        <v>22862.436187568717</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <f>C59*(1+0.00021)^(43)</f>
+        <v>23069.797039579171</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <f>12.84/12</f>
+        <v>1.07</v>
+      </c>
+      <c r="C62">
+        <v>8000</v>
+      </c>
+      <c r="D62">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <f>C62/((1+0.00107)^(2))+D62/((1+0.00107)^(5))-9750</f>
+        <v>9174.2458763168142</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <f>C63*(1+0.00107)^(4)</f>
+        <v>9213.5747151994765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>